<commit_message>
Hero Balance | Inventory Work
- Preliminary balance for all heroes
- trying to fix issue with base items becoming sellable
</commit_message>
<xml_diff>
--- a/balancing/hero_balance.xlsx
+++ b/balancing/hero_balance.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>Hero</t>
   </si>
@@ -183,6 +183,54 @@
   </si>
   <si>
     <t>Dionysus</t>
+  </si>
+  <si>
+    <t>Gilgamesh (m)</t>
+  </si>
+  <si>
+    <t>Gilgamesh</t>
+  </si>
+  <si>
+    <t>Pecos Bill (m)</t>
+  </si>
+  <si>
+    <t>Pecos Bill</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>AGI</t>
+  </si>
+  <si>
+    <t>Quetzalcoatl (m)</t>
+  </si>
+  <si>
+    <t>Quetzalcoatl</t>
+  </si>
+  <si>
+    <t>Robin Hood (m)</t>
+  </si>
+  <si>
+    <t>Robin Hood</t>
+  </si>
+  <si>
+    <t>Sun Wukong (m)</t>
+  </si>
+  <si>
+    <t>Sun Wukong</t>
+  </si>
+  <si>
+    <t>Thor (m)</t>
+  </si>
+  <si>
+    <t>Thor</t>
+  </si>
+  <si>
+    <t>Zeus (m)</t>
+  </si>
+  <si>
+    <t>Zeus</t>
   </si>
 </sst>
 </file>
@@ -387,7 +435,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -415,6 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
@@ -715,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG11"/>
+  <dimension ref="A1:AG25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1424,7 +1473,7 @@
       <c r="C9">
         <v>0.25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E9">
@@ -1650,7 +1699,7 @@
       <c r="C11">
         <v>0.25</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E11">
@@ -1732,6 +1781,1588 @@
         <v>1</v>
       </c>
       <c r="AF11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12">
+        <f>(B5-B13)/B3</f>
+        <v>-23.499999999999986</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:AF12" si="3">(C5-C13)/C3</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>809.28</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>-373.33333333333343</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>1.0999999999999988</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>0.85600000000000009</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>-30.000000000000071</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>265.00000000000006</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="3"/>
+        <v>35.000000000000007</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="3"/>
+        <v>-130.00000000000006</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="3"/>
+        <v>-19.999999999999996</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="3"/>
+        <v>-150</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="3"/>
+        <v>-254.28571428571425</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="3"/>
+        <v>-72.500000000000014</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <f>SUM(B12:AF12)</f>
+        <v>70.216952380952264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <v>3.33</v>
+      </c>
+      <c r="C13">
+        <v>0.25</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13">
+        <v>150</v>
+      </c>
+      <c r="F13">
+        <v>45</v>
+      </c>
+      <c r="H13">
+        <v>1.6</v>
+      </c>
+      <c r="I13">
+        <v>0.33</v>
+      </c>
+      <c r="J13">
+        <v>0.53</v>
+      </c>
+      <c r="K13">
+        <v>800</v>
+      </c>
+      <c r="L13">
+        <v>1145.6189999999999</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13">
+        <v>22</v>
+      </c>
+      <c r="O13">
+        <v>2.5</v>
+      </c>
+      <c r="P13">
+        <v>13</v>
+      </c>
+      <c r="Q13">
+        <v>1.4</v>
+      </c>
+      <c r="R13">
+        <v>22</v>
+      </c>
+      <c r="S13">
+        <v>2.8</v>
+      </c>
+      <c r="T13">
+        <v>315</v>
+      </c>
+      <c r="U13">
+        <v>0.6</v>
+      </c>
+      <c r="V13">
+        <v>200</v>
+      </c>
+      <c r="W13">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="X13">
+        <v>75</v>
+      </c>
+      <c r="Y13">
+        <v>1.5</v>
+      </c>
+      <c r="Z13">
+        <v>1800</v>
+      </c>
+      <c r="AA13">
+        <v>800</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>1</v>
+      </c>
+      <c r="AD13">
+        <v>1</v>
+      </c>
+      <c r="AE13">
+        <v>1</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14">
+        <f>(B5-B15)/B3</f>
+        <v>409.50000000000006</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:AF14" si="4">(C5-C15)/C3</f>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>-990.72</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>759.99999999999989</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>-0.84399999999999975</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>-0.59999999999999942</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f>(L5-L15)*L3</f>
+        <v>-13.087620000000001</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>219.99999999999991</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="4"/>
+        <v>62.5</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>-84.999999999999957</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="4"/>
+        <v>-14.999999999999991</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="4"/>
+        <v>-130.00000000000006</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="4"/>
+        <v>-50</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="4"/>
+        <v>-240</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000022</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <f>SUM(B14:AF14)</f>
+        <v>29.348379999999796</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>-1</v>
+      </c>
+      <c r="C15">
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15">
+        <v>600</v>
+      </c>
+      <c r="F15">
+        <v>28</v>
+      </c>
+      <c r="H15">
+        <v>1.7</v>
+      </c>
+      <c r="I15">
+        <v>0.5</v>
+      </c>
+      <c r="J15">
+        <v>0.6</v>
+      </c>
+      <c r="K15">
+        <v>800</v>
+      </c>
+      <c r="L15">
+        <v>1800</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N15">
+        <v>17</v>
+      </c>
+      <c r="O15">
+        <v>1.5</v>
+      </c>
+      <c r="P15">
+        <v>20</v>
+      </c>
+      <c r="Q15">
+        <v>2.4</v>
+      </c>
+      <c r="R15">
+        <v>22</v>
+      </c>
+      <c r="S15">
+        <v>3.4</v>
+      </c>
+      <c r="T15">
+        <v>290</v>
+      </c>
+      <c r="U15">
+        <v>0.6</v>
+      </c>
+      <c r="V15">
+        <v>200</v>
+      </c>
+      <c r="W15">
+        <v>1.95</v>
+      </c>
+      <c r="X15">
+        <v>75</v>
+      </c>
+      <c r="Y15">
+        <v>1.2</v>
+      </c>
+      <c r="Z15">
+        <v>1800</v>
+      </c>
+      <c r="AA15">
+        <v>800</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <v>1</v>
+      </c>
+      <c r="AE15">
+        <v>1</v>
+      </c>
+      <c r="AF15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16">
+        <f>(B5-B17)/B3</f>
+        <v>209.50000000000003</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:AF16" si="5">(C5-C17)/C3</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="5"/>
+        <v>-990.72</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="5"/>
+        <v>559.99999999999989</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="5"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>-0.34399999999999986</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>5.4</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>(L5-L17)*L3</f>
+        <v>4.912379999999998</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>219.99999999999991</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="5"/>
+        <v>27.499999999999989</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="5"/>
+        <v>115.00000000000003</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="5"/>
+        <v>-59.999999999999986</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="5"/>
+        <v>169.99999999999991</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="5"/>
+        <v>39.999999999999993</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="5"/>
+        <v>-240</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="5"/>
+        <v>-22.500000000000018</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <f>SUM(B16:AF16)</f>
+        <v>88.848379999999722</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0.25</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17">
+        <v>600</v>
+      </c>
+      <c r="F17">
+        <v>31</v>
+      </c>
+      <c r="H17">
+        <v>1.7</v>
+      </c>
+      <c r="I17">
+        <v>0.45</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>800</v>
+      </c>
+      <c r="L17">
+        <v>900</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17">
+        <v>17</v>
+      </c>
+      <c r="O17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P17">
+        <v>16</v>
+      </c>
+      <c r="Q17">
+        <v>3.3</v>
+      </c>
+      <c r="R17">
+        <v>16</v>
+      </c>
+      <c r="S17">
+        <v>1.6</v>
+      </c>
+      <c r="T17">
+        <v>295</v>
+      </c>
+      <c r="U17">
+        <v>0.6</v>
+      </c>
+      <c r="V17">
+        <v>200</v>
+      </c>
+      <c r="W17">
+        <v>1.95</v>
+      </c>
+      <c r="X17">
+        <v>75</v>
+      </c>
+      <c r="Y17">
+        <v>1.3</v>
+      </c>
+      <c r="Z17">
+        <v>1800</v>
+      </c>
+      <c r="AA17">
+        <v>800</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17">
+        <v>1</v>
+      </c>
+      <c r="AD17">
+        <v>1</v>
+      </c>
+      <c r="AE17">
+        <v>1</v>
+      </c>
+      <c r="AF17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18">
+        <f>(B5-B19)/B3</f>
+        <v>409.50000000000006</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:AF18" si="6">(C5-C19)/C3</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="6"/>
+        <v>-990.72</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="6"/>
+        <v>559.99999999999989</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="6"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="6"/>
+        <v>1.1560000000000004</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="6"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>(L5-L19)*L3</f>
+        <v>-1.0876200000000018</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="6"/>
+        <v>169.99999999999991</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="6"/>
+        <v>12.5</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="6"/>
+        <v>165.00000000000003</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="6"/>
+        <v>55</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="6"/>
+        <v>-80.000000000000071</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="6"/>
+        <v>-25</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="6"/>
+        <v>-297.14285714285717</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="6"/>
+        <v>-72.500000000000014</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <f>SUM(B18:AF18)</f>
+        <v>9.2055228571425545</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19">
+        <v>-1</v>
+      </c>
+      <c r="C19">
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19">
+        <v>600</v>
+      </c>
+      <c r="F19">
+        <v>31</v>
+      </c>
+      <c r="H19">
+        <v>1.7</v>
+      </c>
+      <c r="I19">
+        <v>0.3</v>
+      </c>
+      <c r="J19">
+        <v>0.3</v>
+      </c>
+      <c r="K19">
+        <v>800</v>
+      </c>
+      <c r="L19">
+        <v>1200</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N19">
+        <v>18</v>
+      </c>
+      <c r="O19">
+        <v>2.5</v>
+      </c>
+      <c r="P19">
+        <v>15</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>21</v>
+      </c>
+      <c r="S19">
+        <v>2.9</v>
+      </c>
+      <c r="T19">
+        <v>290</v>
+      </c>
+      <c r="U19">
+        <v>0.6</v>
+      </c>
+      <c r="V19">
+        <v>200</v>
+      </c>
+      <c r="W19">
+        <v>2.35</v>
+      </c>
+      <c r="X19">
+        <v>75</v>
+      </c>
+      <c r="Y19">
+        <v>1.5</v>
+      </c>
+      <c r="Z19">
+        <v>1800</v>
+      </c>
+      <c r="AA19">
+        <v>800</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>1</v>
+      </c>
+      <c r="AD19">
+        <v>1</v>
+      </c>
+      <c r="AE19">
+        <v>1</v>
+      </c>
+      <c r="AF19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20">
+        <f>(B5-B21)/B3</f>
+        <v>109.50000000000001</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:AF20" si="7">(C5-C21)/C3</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="7"/>
+        <v>209.27999999999997</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>426.66666666666657</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="7"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="7"/>
+        <v>-0.34399999999999986</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="7"/>
+        <v>3.4</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="7"/>
+        <v>69.999999999999929</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="7"/>
+        <v>-2.4999999999999911</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="7"/>
+        <v>-84.999999999999957</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="7"/>
+        <v>15.000000000000002</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="7"/>
+        <v>-230.00000000000006</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="7"/>
+        <v>-65.000000000000014</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="7"/>
+        <v>-361.42857142857139</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000022</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <f>SUM(B20:AF20)</f>
+        <v>92.174095238094822</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>0.25</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21">
+        <v>300</v>
+      </c>
+      <c r="F21">
+        <v>33</v>
+      </c>
+      <c r="H21">
+        <v>1.7</v>
+      </c>
+      <c r="I21">
+        <v>0.45</v>
+      </c>
+      <c r="J21">
+        <v>0.2</v>
+      </c>
+      <c r="K21">
+        <v>800</v>
+      </c>
+      <c r="L21">
+        <v>1145.6189999999999</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21">
+        <v>20</v>
+      </c>
+      <c r="O21">
+        <v>2.8</v>
+      </c>
+      <c r="P21">
+        <v>20</v>
+      </c>
+      <c r="Q21">
+        <v>1.8</v>
+      </c>
+      <c r="R21">
+        <v>24</v>
+      </c>
+      <c r="S21">
+        <v>3.7</v>
+      </c>
+      <c r="T21">
+        <v>300</v>
+      </c>
+      <c r="U21">
+        <v>0.6</v>
+      </c>
+      <c r="V21">
+        <v>200</v>
+      </c>
+      <c r="W21">
+        <v>2.8</v>
+      </c>
+      <c r="X21">
+        <v>75</v>
+      </c>
+      <c r="Y21">
+        <v>1.2</v>
+      </c>
+      <c r="Z21">
+        <v>1800</v>
+      </c>
+      <c r="AA21">
+        <v>800</v>
+      </c>
+      <c r="AB21">
+        <v>1</v>
+      </c>
+      <c r="AC21">
+        <v>1</v>
+      </c>
+      <c r="AD21">
+        <v>1</v>
+      </c>
+      <c r="AE21">
+        <v>1</v>
+      </c>
+      <c r="AF21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22">
+        <f>(B5-B23)/B3</f>
+        <v>209.50000000000003</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:AF22" si="8">(C5-C23)/C3</f>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="8"/>
+        <v>809.28</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="8"/>
+        <v>-306.6666666666668</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="8"/>
+        <v>-1.8999999999999995</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="8"/>
+        <v>0.15600000000000003</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="8"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="8"/>
+        <v>-30.000000000000071</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="8"/>
+        <v>-22.500000000000007</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="8"/>
+        <v>115.00000000000003</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="8"/>
+        <v>-80.000000000000071</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="8"/>
+        <v>9.9999999999999858</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="8"/>
+        <v>-200</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="8"/>
+        <v>-361.42857142857139</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="8"/>
+        <v>-72.500000000000014</v>
+      </c>
+      <c r="Z22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AG22">
+        <f>SUM(B22:AF22)</f>
+        <v>111.34076190476155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0.25</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23">
+        <v>150</v>
+      </c>
+      <c r="F23">
+        <v>44</v>
+      </c>
+      <c r="H23">
+        <v>1.9</v>
+      </c>
+      <c r="I23">
+        <v>0.4</v>
+      </c>
+      <c r="J23">
+        <v>0.3</v>
+      </c>
+      <c r="K23">
+        <v>800</v>
+      </c>
+      <c r="L23">
+        <v>1145.6189999999999</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N23">
+        <v>22</v>
+      </c>
+      <c r="O23">
+        <v>3.2</v>
+      </c>
+      <c r="P23">
+        <v>16</v>
+      </c>
+      <c r="Q23">
+        <v>1.3</v>
+      </c>
+      <c r="R23">
+        <v>21</v>
+      </c>
+      <c r="S23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T23">
+        <v>320</v>
+      </c>
+      <c r="U23">
+        <v>0.6</v>
+      </c>
+      <c r="V23">
+        <v>200</v>
+      </c>
+      <c r="W23">
+        <v>2.8</v>
+      </c>
+      <c r="X23">
+        <v>75</v>
+      </c>
+      <c r="Y23">
+        <v>1.5</v>
+      </c>
+      <c r="Z23">
+        <v>1800</v>
+      </c>
+      <c r="AA23">
+        <v>800</v>
+      </c>
+      <c r="AB23">
+        <v>1</v>
+      </c>
+      <c r="AC23">
+        <v>1</v>
+      </c>
+      <c r="AD23">
+        <v>1</v>
+      </c>
+      <c r="AE23">
+        <v>1</v>
+      </c>
+      <c r="AF23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24">
+        <f>(B5-B25)/B3</f>
+        <v>209.50000000000003</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:AF24" si="9">(C5-C25)/C3</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="9"/>
+        <v>-990.72</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="9"/>
+        <v>693.33333333333326</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="9"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="9"/>
+        <v>0.65600000000000047</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="9"/>
+        <v>-0.10000000000000009</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f>(L5-L25)*L3</f>
+        <v>0.9123799999999983</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="9"/>
+        <v>119.99999999999993</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="9"/>
+        <v>32.499999999999993</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="9"/>
+        <v>-184.99999999999997</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="9"/>
+        <v>-59.999999999999986</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="9"/>
+        <v>419.99999999999994</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="9"/>
+        <v>-150</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="9"/>
+        <v>-268.57142857142856</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="9"/>
+        <v>2.5000000000000022</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <f>SUM(B24:AF24)</f>
+        <v>-114.88971523809539</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.25</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25">
+        <v>600</v>
+      </c>
+      <c r="F25">
+        <v>29</v>
+      </c>
+      <c r="H25">
+        <v>1.7</v>
+      </c>
+      <c r="I25">
+        <v>0.35</v>
+      </c>
+      <c r="J25">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K25">
+        <v>800</v>
+      </c>
+      <c r="L25">
+        <v>1100</v>
+      </c>
+      <c r="M25" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="N25">
+        <v>19</v>
+      </c>
+      <c r="O25">
+        <v>2.1</v>
+      </c>
+      <c r="P25">
+        <v>22</v>
+      </c>
+      <c r="Q25">
+        <v>3.3</v>
+      </c>
+      <c r="R25">
+        <v>11</v>
+      </c>
+      <c r="S25">
+        <v>1.2</v>
+      </c>
+      <c r="T25">
+        <v>315</v>
+      </c>
+      <c r="U25">
+        <v>0.6</v>
+      </c>
+      <c r="V25">
+        <v>200</v>
+      </c>
+      <c r="W25">
+        <v>2.15</v>
+      </c>
+      <c r="X25">
+        <v>75</v>
+      </c>
+      <c r="Y25">
+        <v>1.2</v>
+      </c>
+      <c r="Z25">
+        <v>1800</v>
+      </c>
+      <c r="AA25">
+        <v>800</v>
+      </c>
+      <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
+        <v>1</v>
+      </c>
+      <c r="AD25">
+        <v>1</v>
+      </c>
+      <c r="AE25">
+        <v>1</v>
+      </c>
+      <c r="AF25">
         <v>1</v>
       </c>
     </row>

</xml_diff>